<commit_message>
Cadastro de Solicitante - incompleto
</commit_message>
<xml_diff>
--- a/Controle.xlsx
+++ b/Controle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kanban" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Backlog</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>Processo Externo - Endereços - Otimizações</t>
+  </si>
+  <si>
+    <t>Testar todas as Pesquisas</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Alta</t>
   </si>
 </sst>
 </file>
@@ -480,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -703,10 +712,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,10 +742,27 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção de erro após merge
</commit_message>
<xml_diff>
--- a/Controle.xlsx
+++ b/Controle.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Backlog</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Alta</t>
+  </si>
+  <si>
+    <t>Exclusão de Entidade de Facturação</t>
   </si>
 </sst>
 </file>
@@ -712,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,6 +766,20 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Processo Externo e atualização da Planilha de Controle
</commit_message>
<xml_diff>
--- a/Controle.xlsx
+++ b/Controle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Kanban" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Backlog</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Importação das Planilhas</t>
   </si>
   <si>
-    <t>Leitura OK. Erro na gravação</t>
-  </si>
-  <si>
     <t>Processo Externo - Endereços - Otimizações</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Exclusão de Entidade de Facturação</t>
+  </si>
+  <si>
+    <t>Verificar data e hora do Histórico: está exibindo 1 dia a mais e não está gravando a hora</t>
   </si>
 </sst>
 </file>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,24 +559,22 @@
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F5" t="s">
@@ -591,7 +589,7 @@
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
@@ -619,7 +617,7 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F8" t="s">
@@ -633,7 +631,7 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
@@ -675,7 +673,7 @@
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F12" t="s">
@@ -715,10 +713,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -760,10 +758,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -774,12 +772,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>